<commit_message>
final update of capstone (~12.18)
</commit_message>
<xml_diff>
--- a/DB DATA/성격유형분류_하나성빈 합친거.xlsx
+++ b/DB DATA/성격유형분류_하나성빈 합친거.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMINI~1\DOCUME~1\카카오~1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adelv\github-sourcetree\MJ\DB DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8008714E-6DEE-4FA5-ABFE-5ABC47353682}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="2805" windowWidth="15990" windowHeight="9315" xr2:uid="{1F52A049-A1BD-4896-8456-CD5D4B78C7C4}"/>
+    <workbookView xWindow="4440" yWindow="2805" windowWidth="15990" windowHeight="9315"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="846">
   <si>
     <t>독립운동가</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2238,14 +2237,1159 @@
   </si>
   <si>
     <t>계보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>첩보원</t>
+  </si>
+  <si>
+    <t>수렵인</t>
+  </si>
+  <si>
+    <t>신화</t>
+  </si>
+  <si>
+    <t>운동인</t>
+  </si>
+  <si>
+    <t>어부</t>
+  </si>
+  <si>
+    <t>소장가</t>
+  </si>
+  <si>
+    <t>연루자</t>
+  </si>
+  <si>
+    <t>지도자</t>
+  </si>
+  <si>
+    <t>영화인</t>
+  </si>
+  <si>
+    <t>장구</t>
+  </si>
+  <si>
+    <t>이론가</t>
+  </si>
+  <si>
+    <t>정치인</t>
+  </si>
+  <si>
+    <t>은행가</t>
+  </si>
+  <si>
+    <t>유학</t>
+  </si>
+  <si>
+    <t>요리사</t>
+  </si>
+  <si>
+    <t>연구자</t>
+  </si>
+  <si>
+    <t>중국</t>
+  </si>
+  <si>
+    <t>원화*</t>
+  </si>
+  <si>
+    <t>피아노</t>
+  </si>
+  <si>
+    <t>평론가</t>
+  </si>
+  <si>
+    <t>첼로</t>
+  </si>
+  <si>
+    <t>극인</t>
+  </si>
+  <si>
+    <t>퉁소</t>
+  </si>
+  <si>
+    <t>피리</t>
+  </si>
+  <si>
+    <t>트럼본</t>
+  </si>
+  <si>
+    <t>일본</t>
+  </si>
+  <si>
+    <t>해금</t>
+  </si>
+  <si>
+    <t>무용가</t>
+  </si>
+  <si>
+    <t>수조각승*</t>
+  </si>
+  <si>
+    <t>조작가*</t>
+  </si>
+  <si>
+    <t>콘트라바스</t>
+  </si>
+  <si>
+    <t>자연</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자연인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>속세</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자급자족</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>외국</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유학</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>여행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중국</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">호더 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수집</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수집가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물건</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구매</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>골동품</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지름신</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>텅장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체육</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>운동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>헬스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스포츠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>올림픽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>월드컵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체대생</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>달리기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>요가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미신</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그리스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>로마</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>신</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>여신</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제우스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이야기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구전</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>고전</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레전드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물고기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바람</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제주도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>닻</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>낚시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>그물</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>게</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대통령</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장관</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공무원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>왕</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>족장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>산</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>농사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>원시인</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구시대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리더</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>팀플</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>캐리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>버스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관련</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관련자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공범</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공조</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공조자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연루</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">영화 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>씨지비</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>메가박스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>롯시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>롯데시네마</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개봉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>블록버스터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>독립영화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>배우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>감독</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연관</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연관자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공조자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공범자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연구실</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연구소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과학</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공학</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>논문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>실험</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>과학자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대학원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>석사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금수저</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해외</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유학</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해외취업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>워홀</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>워킹홀리데이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>학문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>여행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>은행</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>국민</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>하나</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금융</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대출</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>저축</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>투자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주식</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>돈</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>백종원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>요리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한식</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중식</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일식</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>즉석음식</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>볶음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>부엌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>식당</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>요식업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이론</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>책</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개념</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연구자</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>논문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사상</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>의견</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전공책</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전공</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>음악</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>악기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전통음악</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전통악기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>드럼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>북</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>국악</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연주</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연주가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>국회의원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>국회</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>의원</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>탄핵</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시위</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>입법</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>국회의사당</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>선거</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>촛불</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조작단</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>계획</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>음모</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>여론</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>음해</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뒷공작</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>소문</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>언플</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>홍콩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동방</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아시아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상하이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>베이징</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>동아시아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시진핑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연극</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>극장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>극단</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공연</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뮤지컬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오페라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연출</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무대</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">스파이 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>산업스파이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>유출</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뒷통수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>첩보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>첩보물</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>판극</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>판소리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>음악</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>오케스트라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바이올린</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비올라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현악기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>예술</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>예고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>출판사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미슐랭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평론</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비판</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평론집</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비평</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>후기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리뷰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>리뷰어</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서양악기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">악기 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>첼로</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>바이올린</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>베이스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>활</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>악단</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>퉁애</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관악기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>죽부악기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당악기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대나무</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>단소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대금</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>민속음악</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>국악</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관악기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금관악기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공기울림악기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>트렘펫</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>튜바</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>호른</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기명악기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공연</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>귀족</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>관악기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>해금</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>장구</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가야금</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플루트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피아노</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>건반</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>밴드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피아니스트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>독주</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>감미</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이루마</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>찰현악기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>악기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>거문고</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아쟁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전통</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한국</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>당나라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>현대무용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>발레</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>비보이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무용수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>한국무용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사회무용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>춤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>노래</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>연습실</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아시아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>역사</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>도쿄</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>외국</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>후쿠오카</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제이팝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>불매</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무역</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2260,6 +3404,12 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2285,21 +3435,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="표준_Sheet1" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2610,11 +3767,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEE4E206-09C7-4308-BA3E-484A562A81FE}">
-  <dimension ref="A1:L63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="L47" sqref="L47"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="K94" sqref="K94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4713,8 +5870,1048 @@
       <c r="A63" s="1" t="s">
         <v>305</v>
       </c>
+      <c r="B63" t="s">
+        <v>587</v>
+      </c>
+      <c r="C63" t="s">
+        <v>588</v>
+      </c>
+      <c r="D63" t="s">
+        <v>589</v>
+      </c>
+      <c r="E63" t="s">
+        <v>588</v>
+      </c>
+      <c r="F63" t="s">
+        <v>590</v>
+      </c>
       <c r="L63" t="s">
         <v>329</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="B64" t="s">
+        <v>583</v>
+      </c>
+      <c r="C64" t="s">
+        <v>584</v>
+      </c>
+      <c r="D64" t="s">
+        <v>585</v>
+      </c>
+      <c r="E64" t="s">
+        <v>586</v>
+      </c>
+      <c r="F64" t="s">
+        <v>636</v>
+      </c>
+      <c r="G64" t="s">
+        <v>621</v>
+      </c>
+      <c r="H64" t="s">
+        <v>637</v>
+      </c>
+      <c r="I64" t="s">
+        <v>628</v>
+      </c>
+      <c r="J64" t="s">
+        <v>638</v>
+      </c>
+      <c r="K64" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="B65" t="s">
+        <v>591</v>
+      </c>
+      <c r="C65" t="s">
+        <v>592</v>
+      </c>
+      <c r="D65" t="s">
+        <v>593</v>
+      </c>
+      <c r="E65" t="s">
+        <v>594</v>
+      </c>
+      <c r="F65" t="s">
+        <v>595</v>
+      </c>
+      <c r="G65" t="s">
+        <v>596</v>
+      </c>
+      <c r="H65" t="s">
+        <v>597</v>
+      </c>
+      <c r="I65" t="s">
+        <v>598</v>
+      </c>
+      <c r="J65" t="s">
+        <v>599</v>
+      </c>
+      <c r="K65" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A67" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="B67" t="s">
+        <v>601</v>
+      </c>
+      <c r="C67" t="s">
+        <v>602</v>
+      </c>
+      <c r="D67" t="s">
+        <v>603</v>
+      </c>
+      <c r="E67" t="s">
+        <v>604</v>
+      </c>
+      <c r="F67" t="s">
+        <v>605</v>
+      </c>
+      <c r="G67" t="s">
+        <v>606</v>
+      </c>
+      <c r="H67" t="s">
+        <v>607</v>
+      </c>
+      <c r="I67" t="s">
+        <v>608</v>
+      </c>
+      <c r="J67" t="s">
+        <v>609</v>
+      </c>
+      <c r="K67" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A68" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="B68" t="s">
+        <v>611</v>
+      </c>
+      <c r="C68" t="s">
+        <v>612</v>
+      </c>
+      <c r="D68" t="s">
+        <v>613</v>
+      </c>
+      <c r="E68" t="s">
+        <v>614</v>
+      </c>
+      <c r="F68" t="s">
+        <v>615</v>
+      </c>
+      <c r="G68" t="s">
+        <v>616</v>
+      </c>
+      <c r="H68" t="s">
+        <v>617</v>
+      </c>
+      <c r="I68" t="s">
+        <v>618</v>
+      </c>
+      <c r="J68" t="s">
+        <v>619</v>
+      </c>
+      <c r="K68" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A69" s="2" t="s">
+        <v>556</v>
+      </c>
+      <c r="B69" t="s">
+        <v>621</v>
+      </c>
+      <c r="C69" t="s">
+        <v>622</v>
+      </c>
+      <c r="D69" t="s">
+        <v>623</v>
+      </c>
+      <c r="E69" t="s">
+        <v>624</v>
+      </c>
+      <c r="F69" t="s">
+        <v>625</v>
+      </c>
+      <c r="G69" t="s">
+        <v>626</v>
+      </c>
+      <c r="H69" t="s">
+        <v>627</v>
+      </c>
+      <c r="I69" t="s">
+        <v>628</v>
+      </c>
+      <c r="J69" t="s">
+        <v>629</v>
+      </c>
+      <c r="K69" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="B70" t="s">
+        <v>631</v>
+      </c>
+      <c r="C70" t="s">
+        <v>632</v>
+      </c>
+      <c r="D70" t="s">
+        <v>633</v>
+      </c>
+      <c r="E70" t="s">
+        <v>634</v>
+      </c>
+      <c r="F70" t="s">
+        <v>635</v>
+      </c>
+      <c r="G70" t="s">
+        <v>640</v>
+      </c>
+      <c r="H70" t="s">
+        <v>641</v>
+      </c>
+      <c r="I70" t="s">
+        <v>642</v>
+      </c>
+      <c r="J70" t="s">
+        <v>643</v>
+      </c>
+      <c r="K70" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="B71" t="s">
+        <v>645</v>
+      </c>
+      <c r="C71" t="s">
+        <v>646</v>
+      </c>
+      <c r="D71" t="s">
+        <v>647</v>
+      </c>
+      <c r="E71" t="s">
+        <v>648</v>
+      </c>
+      <c r="F71" t="s">
+        <v>649</v>
+      </c>
+      <c r="G71" t="s">
+        <v>650</v>
+      </c>
+      <c r="H71" t="s">
+        <v>661</v>
+      </c>
+      <c r="I71" t="s">
+        <v>662</v>
+      </c>
+      <c r="J71" t="s">
+        <v>663</v>
+      </c>
+      <c r="K71" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="B72" t="s">
+        <v>651</v>
+      </c>
+      <c r="C72" t="s">
+        <v>652</v>
+      </c>
+      <c r="D72" t="s">
+        <v>653</v>
+      </c>
+      <c r="E72" t="s">
+        <v>654</v>
+      </c>
+      <c r="F72" t="s">
+        <v>655</v>
+      </c>
+      <c r="G72" t="s">
+        <v>656</v>
+      </c>
+      <c r="H72" t="s">
+        <v>660</v>
+      </c>
+      <c r="I72" t="s">
+        <v>659</v>
+      </c>
+      <c r="J72" t="s">
+        <v>657</v>
+      </c>
+      <c r="K72" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="B73" t="s">
+        <v>665</v>
+      </c>
+      <c r="C73" t="s">
+        <v>666</v>
+      </c>
+      <c r="D73" t="s">
+        <v>667</v>
+      </c>
+      <c r="E73" t="s">
+        <v>668</v>
+      </c>
+      <c r="F73" t="s">
+        <v>669</v>
+      </c>
+      <c r="G73" t="s">
+        <v>673</v>
+      </c>
+      <c r="H73" t="s">
+        <v>670</v>
+      </c>
+      <c r="I73" t="s">
+        <v>671</v>
+      </c>
+      <c r="J73" t="s">
+        <v>672</v>
+      </c>
+      <c r="K73" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="B75" t="s">
+        <v>675</v>
+      </c>
+      <c r="C75" t="s">
+        <v>676</v>
+      </c>
+      <c r="D75" t="s">
+        <v>677</v>
+      </c>
+      <c r="E75" t="s">
+        <v>678</v>
+      </c>
+      <c r="F75" t="s">
+        <v>679</v>
+      </c>
+      <c r="G75" t="s">
+        <v>680</v>
+      </c>
+      <c r="H75" t="s">
+        <v>681</v>
+      </c>
+      <c r="I75" t="s">
+        <v>682</v>
+      </c>
+      <c r="J75" t="s">
+        <v>683</v>
+      </c>
+      <c r="K75" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A76" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="B76" t="s">
+        <v>685</v>
+      </c>
+      <c r="C76" t="s">
+        <v>686</v>
+      </c>
+      <c r="D76" t="s">
+        <v>687</v>
+      </c>
+      <c r="E76" t="s">
+        <v>688</v>
+      </c>
+      <c r="F76" t="s">
+        <v>689</v>
+      </c>
+      <c r="G76" t="s">
+        <v>690</v>
+      </c>
+      <c r="H76" t="s">
+        <v>691</v>
+      </c>
+      <c r="I76" t="s">
+        <v>692</v>
+      </c>
+      <c r="J76" t="s">
+        <v>693</v>
+      </c>
+      <c r="K76" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A77" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="B77" t="s">
+        <v>695</v>
+      </c>
+      <c r="C77" t="s">
+        <v>696</v>
+      </c>
+      <c r="D77" t="s">
+        <v>697</v>
+      </c>
+      <c r="E77" t="s">
+        <v>698</v>
+      </c>
+      <c r="F77" t="s">
+        <v>699</v>
+      </c>
+      <c r="G77" t="s">
+        <v>700</v>
+      </c>
+      <c r="H77" t="s">
+        <v>701</v>
+      </c>
+      <c r="I77" t="s">
+        <v>702</v>
+      </c>
+      <c r="J77" t="s">
+        <v>703</v>
+      </c>
+      <c r="K77" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A78" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="B78" t="s">
+        <v>705</v>
+      </c>
+      <c r="C78" t="s">
+        <v>706</v>
+      </c>
+      <c r="D78" t="s">
+        <v>707</v>
+      </c>
+      <c r="E78" t="s">
+        <v>708</v>
+      </c>
+      <c r="F78" t="s">
+        <v>709</v>
+      </c>
+      <c r="G78" t="s">
+        <v>710</v>
+      </c>
+      <c r="H78" t="s">
+        <v>711</v>
+      </c>
+      <c r="I78" t="s">
+        <v>712</v>
+      </c>
+      <c r="J78" t="s">
+        <v>713</v>
+      </c>
+      <c r="K78" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A79" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="B79" t="s">
+        <v>715</v>
+      </c>
+      <c r="C79" t="s">
+        <v>716</v>
+      </c>
+      <c r="D79" t="s">
+        <v>717</v>
+      </c>
+      <c r="E79" t="s">
+        <v>718</v>
+      </c>
+      <c r="F79" t="s">
+        <v>719</v>
+      </c>
+      <c r="G79" t="s">
+        <v>720</v>
+      </c>
+      <c r="H79" t="s">
+        <v>721</v>
+      </c>
+      <c r="I79" t="s">
+        <v>722</v>
+      </c>
+      <c r="J79" t="s">
+        <v>723</v>
+      </c>
+      <c r="K79" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A80" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="B80" t="s">
+        <v>631</v>
+      </c>
+      <c r="C80" t="s">
+        <v>725</v>
+      </c>
+      <c r="D80" t="s">
+        <v>726</v>
+      </c>
+      <c r="E80" t="s">
+        <v>727</v>
+      </c>
+      <c r="F80" t="s">
+        <v>728</v>
+      </c>
+      <c r="G80" t="s">
+        <v>729</v>
+      </c>
+      <c r="H80" t="s">
+        <v>730</v>
+      </c>
+      <c r="I80" t="s">
+        <v>731</v>
+      </c>
+      <c r="J80" t="s">
+        <v>732</v>
+      </c>
+      <c r="K80" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A81" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="B81" t="s">
+        <v>734</v>
+      </c>
+      <c r="C81" t="s">
+        <v>735</v>
+      </c>
+      <c r="D81" t="s">
+        <v>736</v>
+      </c>
+      <c r="E81" t="s">
+        <v>737</v>
+      </c>
+      <c r="F81" t="s">
+        <v>738</v>
+      </c>
+      <c r="G81" t="s">
+        <v>739</v>
+      </c>
+      <c r="H81" t="s">
+        <v>740</v>
+      </c>
+      <c r="I81" t="s">
+        <v>741</v>
+      </c>
+      <c r="J81" t="s">
+        <v>742</v>
+      </c>
+      <c r="K81" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A82" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="B82" t="s">
+        <v>587</v>
+      </c>
+      <c r="C82" t="s">
+        <v>744</v>
+      </c>
+      <c r="D82" t="s">
+        <v>745</v>
+      </c>
+      <c r="E82" t="s">
+        <v>746</v>
+      </c>
+      <c r="F82" t="s">
+        <v>590</v>
+      </c>
+      <c r="G82" t="s">
+        <v>747</v>
+      </c>
+      <c r="H82" t="s">
+        <v>748</v>
+      </c>
+      <c r="I82" t="s">
+        <v>749</v>
+      </c>
+      <c r="J82" t="s">
+        <v>589</v>
+      </c>
+      <c r="K82" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A83" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="B83" t="s">
+        <v>751</v>
+      </c>
+      <c r="C83" t="s">
+        <v>752</v>
+      </c>
+      <c r="D83" t="s">
+        <v>753</v>
+      </c>
+      <c r="E83" t="s">
+        <v>754</v>
+      </c>
+      <c r="F83" t="s">
+        <v>755</v>
+      </c>
+      <c r="G83" t="s">
+        <v>756</v>
+      </c>
+      <c r="H83" t="s">
+        <v>757</v>
+      </c>
+      <c r="I83" t="s">
+        <v>758</v>
+      </c>
+      <c r="J83" t="s">
+        <v>765</v>
+      </c>
+      <c r="K83" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A84" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="B84" t="s">
+        <v>759</v>
+      </c>
+      <c r="C84" t="s">
+        <v>735</v>
+      </c>
+      <c r="D84" t="s">
+        <v>739</v>
+      </c>
+      <c r="E84" t="s">
+        <v>742</v>
+      </c>
+      <c r="F84" t="s">
+        <v>741</v>
+      </c>
+      <c r="G84" t="s">
+        <v>760</v>
+      </c>
+      <c r="H84" t="s">
+        <v>761</v>
+      </c>
+      <c r="I84" t="s">
+        <v>762</v>
+      </c>
+      <c r="J84" t="s">
+        <v>763</v>
+      </c>
+      <c r="K84" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="B85" t="s">
+        <v>767</v>
+      </c>
+      <c r="C85" t="s">
+        <v>717</v>
+      </c>
+      <c r="D85" t="s">
+        <v>768</v>
+      </c>
+      <c r="E85" t="s">
+        <v>769</v>
+      </c>
+      <c r="F85" t="s">
+        <v>770</v>
+      </c>
+      <c r="G85" t="s">
+        <v>771</v>
+      </c>
+      <c r="H85" t="s">
+        <v>723</v>
+      </c>
+      <c r="I85" t="s">
+        <v>754</v>
+      </c>
+      <c r="J85" t="s">
+        <v>773</v>
+      </c>
+      <c r="K85" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="B86" t="s">
+        <v>774</v>
+      </c>
+      <c r="C86" t="s">
+        <v>775</v>
+      </c>
+      <c r="D86" t="s">
+        <v>776</v>
+      </c>
+      <c r="E86" t="s">
+        <v>777</v>
+      </c>
+      <c r="F86" t="s">
+        <v>778</v>
+      </c>
+      <c r="G86" t="s">
+        <v>706</v>
+      </c>
+      <c r="H86" t="s">
+        <v>779</v>
+      </c>
+      <c r="I86" t="s">
+        <v>780</v>
+      </c>
+      <c r="J86" t="s">
+        <v>781</v>
+      </c>
+      <c r="K86" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="B87" t="s">
+        <v>771</v>
+      </c>
+      <c r="C87" t="s">
+        <v>783</v>
+      </c>
+      <c r="D87" t="s">
+        <v>784</v>
+      </c>
+      <c r="E87" t="s">
+        <v>785</v>
+      </c>
+      <c r="F87" t="s">
+        <v>770</v>
+      </c>
+      <c r="G87" t="s">
+        <v>786</v>
+      </c>
+      <c r="H87" t="s">
+        <v>787</v>
+      </c>
+      <c r="I87" t="s">
+        <v>788</v>
+      </c>
+      <c r="J87" t="s">
+        <v>789</v>
+      </c>
+      <c r="K87" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A88" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="B88" t="s">
+        <v>790</v>
+      </c>
+      <c r="C88" t="s">
+        <v>791</v>
+      </c>
+      <c r="D88" t="s">
+        <v>717</v>
+      </c>
+      <c r="E88" t="s">
+        <v>792</v>
+      </c>
+      <c r="F88" t="s">
+        <v>793</v>
+      </c>
+      <c r="G88" t="s">
+        <v>794</v>
+      </c>
+      <c r="H88" t="s">
+        <v>795</v>
+      </c>
+      <c r="I88" t="s">
+        <v>796</v>
+      </c>
+      <c r="J88" t="s">
+        <v>797</v>
+      </c>
+      <c r="K88" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A89" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="B89" t="s">
+        <v>799</v>
+      </c>
+      <c r="C89" t="s">
+        <v>800</v>
+      </c>
+      <c r="D89" t="s">
+        <v>801</v>
+      </c>
+      <c r="E89" t="s">
+        <v>802</v>
+      </c>
+      <c r="F89" t="s">
+        <v>803</v>
+      </c>
+      <c r="G89" t="s">
+        <v>804</v>
+      </c>
+      <c r="H89" t="s">
+        <v>805</v>
+      </c>
+      <c r="I89" t="s">
+        <v>768</v>
+      </c>
+      <c r="J89" t="s">
+        <v>806</v>
+      </c>
+      <c r="K89" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A90" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="B90" t="s">
+        <v>717</v>
+      </c>
+      <c r="C90" t="s">
+        <v>722</v>
+      </c>
+      <c r="D90" t="s">
+        <v>808</v>
+      </c>
+      <c r="E90" t="s">
+        <v>809</v>
+      </c>
+      <c r="F90" t="s">
+        <v>810</v>
+      </c>
+      <c r="G90" t="s">
+        <v>811</v>
+      </c>
+      <c r="H90" t="s">
+        <v>794</v>
+      </c>
+      <c r="I90" t="s">
+        <v>814</v>
+      </c>
+      <c r="J90" t="s">
+        <v>795</v>
+      </c>
+      <c r="K90" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A91" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="B91" t="s">
+        <v>813</v>
+      </c>
+      <c r="C91" t="s">
+        <v>815</v>
+      </c>
+      <c r="D91" t="s">
+        <v>816</v>
+      </c>
+      <c r="E91" t="s">
+        <v>767</v>
+      </c>
+      <c r="F91" t="s">
+        <v>717</v>
+      </c>
+      <c r="G91" t="s">
+        <v>817</v>
+      </c>
+      <c r="H91" t="s">
+        <v>754</v>
+      </c>
+      <c r="I91" t="s">
+        <v>818</v>
+      </c>
+      <c r="J91" t="s">
+        <v>819</v>
+      </c>
+      <c r="K91" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="B92" t="s">
+        <v>722</v>
+      </c>
+      <c r="C92" t="s">
+        <v>809</v>
+      </c>
+      <c r="D92" t="s">
+        <v>821</v>
+      </c>
+      <c r="E92" t="s">
+        <v>822</v>
+      </c>
+      <c r="F92" t="s">
+        <v>823</v>
+      </c>
+      <c r="G92" t="s">
+        <v>814</v>
+      </c>
+      <c r="H92" t="s">
+        <v>824</v>
+      </c>
+      <c r="I92" t="s">
+        <v>825</v>
+      </c>
+      <c r="J92" t="s">
+        <v>826</v>
+      </c>
+      <c r="K92" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A93" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="B93" t="s">
+        <v>828</v>
+      </c>
+      <c r="C93" t="s">
+        <v>829</v>
+      </c>
+      <c r="D93" t="s">
+        <v>830</v>
+      </c>
+      <c r="E93" t="s">
+        <v>831</v>
+      </c>
+      <c r="F93" t="s">
+        <v>832</v>
+      </c>
+      <c r="G93" t="s">
+        <v>833</v>
+      </c>
+      <c r="H93" t="s">
+        <v>834</v>
+      </c>
+      <c r="I93" t="s">
+        <v>835</v>
+      </c>
+      <c r="J93" t="s">
+        <v>836</v>
+      </c>
+      <c r="K93" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A94" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="B94" t="s">
+        <v>749</v>
+      </c>
+      <c r="C94" t="s">
+        <v>838</v>
+      </c>
+      <c r="D94" t="s">
+        <v>589</v>
+      </c>
+      <c r="E94" t="s">
+        <v>839</v>
+      </c>
+      <c r="F94" t="s">
+        <v>840</v>
+      </c>
+      <c r="G94" t="s">
+        <v>841</v>
+      </c>
+      <c r="H94" t="s">
+        <v>842</v>
+      </c>
+      <c r="I94" t="s">
+        <v>843</v>
+      </c>
+      <c r="J94" t="s">
+        <v>844</v>
+      </c>
+      <c r="K94" t="s">
+        <v>845</v>
       </c>
     </row>
   </sheetData>

</xml_diff>